<commit_message>
Add data format id to table columns if data format is consistent.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFColorScaleLowHigh.xlsx
@@ -72,15 +72,6 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="1">
-    <x:dxf>
-      <x:font/>
-      <x:fill>
-        <x:patternFill/>
-      </x:fill>
-      <x:border/>
-    </x:dxf>
-  </x:dxfs>
 </x:styleSheet>
 </file>
 

</xml_diff>